<commit_message>
create file and sheet if not exist
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI Projects\MIDI_Factory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B06088-CBEC-475E-93D6-0E9E69AF459E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BDF6E3-9987-49D9-9798-D23AAE4BB6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4185" yWindow="-10200" windowWidth="20490" windowHeight="9750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1500" yWindow="-10710" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test" sheetId="7" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="9" r:id="rId1"/>
+    <sheet name="test" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="25">
   <si>
     <t>note</t>
   </si>
@@ -218,6 +219,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DF606CD9-9FB2-4B13-80D3-6B2EE810FDEE}" name="MyTable" displayName="MyTable" ref="A1:G184" totalsRowShown="0">
+  <autoFilter ref="A1:G184" xr:uid="{DF606CD9-9FB2-4B13-80D3-6B2EE810FDEE}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{A4B06106-F535-4F44-9117-85ED31AD409F}" name=" "/>
+    <tableColumn id="2" xr3:uid="{09F42CC6-6E1A-4EB2-83D9-EE46FBA56400}" name="note"/>
+    <tableColumn id="3" xr3:uid="{856DD3D5-4CDF-4B8B-AC8D-6F179864F7B1}" name="interval"/>
+    <tableColumn id="4" xr3:uid="{CD3196B1-A477-427F-8567-B2D039404256}" name="note_start_time"/>
+    <tableColumn id="5" xr3:uid="{931D4E04-1AAF-44B3-B4B7-8441F8E2D2DB}" name="duration"/>
+    <tableColumn id="6" xr3:uid="{C2B2A913-570F-49C7-9F4F-641169AEF22F}" name="slur"/>
+    <tableColumn id="7" xr3:uid="{EEE8727A-F886-4C84-9B9B-29405E531AD2}" name="velocity"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="136" xr:uid="{C32C5546-0D5C-4BFB-B7D2-24A59E2FA6B8}" name="MyTable" displayName="MyTable_1" ref="A1:M184" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M184" xr:uid="{C32C5546-0D5C-4BFB-B7D2-24A59E2FA6B8}"/>
   <tableColumns count="13">
@@ -525,10 +542,4108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD71C912-69CF-4936-85E5-637E7C408852}">
+  <dimension ref="A1:G184"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G184"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>384</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>384</v>
+      </c>
+      <c r="E3">
+        <v>96</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>52</v>
+      </c>
+      <c r="D4">
+        <v>480</v>
+      </c>
+      <c r="E4">
+        <v>144</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>55</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>624</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>672</v>
+      </c>
+      <c r="E6">
+        <v>96</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>768</v>
+      </c>
+      <c r="E7">
+        <v>384</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>1152</v>
+      </c>
+      <c r="E8">
+        <v>48</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>51.5</v>
+      </c>
+      <c r="C9">
+        <v>3.5</v>
+      </c>
+      <c r="D9">
+        <v>1200</v>
+      </c>
+      <c r="E9">
+        <v>192</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>3.5</v>
+      </c>
+      <c r="D10">
+        <v>1392</v>
+      </c>
+      <c r="E10">
+        <v>48</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1440</v>
+      </c>
+      <c r="E11">
+        <v>96</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>-12</v>
+      </c>
+      <c r="D12">
+        <v>1536</v>
+      </c>
+      <c r="E12">
+        <v>48</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>52</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1584</v>
+      </c>
+      <c r="E13">
+        <v>96</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>55</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>1680</v>
+      </c>
+      <c r="E14">
+        <v>144</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1824</v>
+      </c>
+      <c r="E15">
+        <v>96</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>48</v>
+      </c>
+      <c r="C16">
+        <v>-12</v>
+      </c>
+      <c r="D16">
+        <v>1920</v>
+      </c>
+      <c r="E16">
+        <v>72</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>52</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>1992</v>
+      </c>
+      <c r="E17">
+        <v>120</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>2112</v>
+      </c>
+      <c r="E18">
+        <v>96</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>60</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>2208</v>
+      </c>
+      <c r="E19">
+        <v>48</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>48</v>
+      </c>
+      <c r="C20">
+        <v>-12</v>
+      </c>
+      <c r="D20">
+        <v>2256</v>
+      </c>
+      <c r="E20">
+        <v>48</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>48</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>2304</v>
+      </c>
+      <c r="E21">
+        <v>96</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>2400</v>
+      </c>
+      <c r="E22">
+        <v>48</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>55</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>2448</v>
+      </c>
+      <c r="E23">
+        <v>144</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>60</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>2592</v>
+      </c>
+      <c r="E24">
+        <v>96</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>48</v>
+      </c>
+      <c r="C25">
+        <v>-12</v>
+      </c>
+      <c r="D25">
+        <v>2688</v>
+      </c>
+      <c r="E25">
+        <v>96</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>2784</v>
+      </c>
+      <c r="E26">
+        <v>96</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>55</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>2880</v>
+      </c>
+      <c r="E27">
+        <v>96</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>60</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>2976</v>
+      </c>
+      <c r="E28">
+        <v>96</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>3072</v>
+      </c>
+      <c r="E29">
+        <v>384</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <v>3456</v>
+      </c>
+      <c r="E30">
+        <v>384</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>3840</v>
+      </c>
+      <c r="E31">
+        <v>96</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>52</v>
+      </c>
+      <c r="D32">
+        <v>3936</v>
+      </c>
+      <c r="E32">
+        <v>96</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>55</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>4032</v>
+      </c>
+      <c r="E33">
+        <v>96</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>60</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>4128</v>
+      </c>
+      <c r="E34">
+        <v>96</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>48</v>
+      </c>
+      <c r="C35">
+        <v>-12</v>
+      </c>
+      <c r="D35">
+        <v>4224</v>
+      </c>
+      <c r="E35">
+        <v>96</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>52</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>4320</v>
+      </c>
+      <c r="E36">
+        <v>96</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>55</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>4416</v>
+      </c>
+      <c r="E37">
+        <v>96</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>60</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>4512</v>
+      </c>
+      <c r="E38">
+        <v>96</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>48</v>
+      </c>
+      <c r="C39">
+        <v>-12</v>
+      </c>
+      <c r="D39">
+        <v>4608</v>
+      </c>
+      <c r="E39">
+        <v>96</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>52</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>4704</v>
+      </c>
+      <c r="E40">
+        <v>96</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>55</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>4800</v>
+      </c>
+      <c r="E41">
+        <v>96</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>60</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>4896</v>
+      </c>
+      <c r="E42">
+        <v>96</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>48</v>
+      </c>
+      <c r="C43">
+        <v>-12</v>
+      </c>
+      <c r="D43">
+        <v>4992</v>
+      </c>
+      <c r="E43">
+        <v>96</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>52</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>5088</v>
+      </c>
+      <c r="E44">
+        <v>96</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>55</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>5184</v>
+      </c>
+      <c r="E45">
+        <v>96</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>60</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>5280</v>
+      </c>
+      <c r="E46">
+        <v>96</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>48</v>
+      </c>
+      <c r="C47">
+        <v>-12</v>
+      </c>
+      <c r="D47">
+        <v>5376</v>
+      </c>
+      <c r="E47">
+        <v>96</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="D48">
+        <v>5472</v>
+      </c>
+      <c r="E48">
+        <v>192</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>56</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <v>5664</v>
+      </c>
+      <c r="E49">
+        <v>48</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="D50">
+        <v>5712</v>
+      </c>
+      <c r="E50">
+        <v>48</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="D51">
+        <v>5760</v>
+      </c>
+      <c r="E51">
+        <v>288</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>60</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>6048</v>
+      </c>
+      <c r="E52">
+        <v>96</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>48</v>
+      </c>
+      <c r="C53">
+        <v>-12</v>
+      </c>
+      <c r="D53">
+        <v>6144</v>
+      </c>
+      <c r="E53">
+        <v>96</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>52</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>6240</v>
+      </c>
+      <c r="E54">
+        <v>96</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>55</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>6336</v>
+      </c>
+      <c r="E55">
+        <v>96</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+      <c r="D56">
+        <v>6432</v>
+      </c>
+      <c r="E56">
+        <v>96</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>48</v>
+      </c>
+      <c r="C57">
+        <v>-12</v>
+      </c>
+      <c r="D57">
+        <v>6528</v>
+      </c>
+      <c r="E57">
+        <v>96</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="D58">
+        <v>6624</v>
+      </c>
+      <c r="E58">
+        <v>192</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>12</v>
+      </c>
+      <c r="D59">
+        <v>6816</v>
+      </c>
+      <c r="E59">
+        <v>96</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>48</v>
+      </c>
+      <c r="C60">
+        <v>-12</v>
+      </c>
+      <c r="D60">
+        <v>6912</v>
+      </c>
+      <c r="E60">
+        <v>96</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>52</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <v>7008</v>
+      </c>
+      <c r="E61">
+        <v>96</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>55</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>7104</v>
+      </c>
+      <c r="E62">
+        <v>96</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>60</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>7200</v>
+      </c>
+      <c r="E63">
+        <v>96</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="D64">
+        <v>7296</v>
+      </c>
+      <c r="E64">
+        <v>192</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>55</v>
+      </c>
+      <c r="C65">
+        <v>-5</v>
+      </c>
+      <c r="D65">
+        <v>7488</v>
+      </c>
+      <c r="E65">
+        <v>96</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>60</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>7584</v>
+      </c>
+      <c r="E66">
+        <v>96</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>48</v>
+      </c>
+      <c r="C67">
+        <v>-12</v>
+      </c>
+      <c r="D67">
+        <v>7680</v>
+      </c>
+      <c r="E67">
+        <v>96</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="D68">
+        <v>7776</v>
+      </c>
+      <c r="E68">
+        <v>288</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>48</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>8064</v>
+      </c>
+      <c r="E69">
+        <v>96</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="D70">
+        <v>8160</v>
+      </c>
+      <c r="E70">
+        <v>288</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>48</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>8448</v>
+      </c>
+      <c r="E71">
+        <v>96</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>52</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>8544</v>
+      </c>
+      <c r="E72">
+        <v>96</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>55</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73">
+        <v>8640</v>
+      </c>
+      <c r="E73">
+        <v>96</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>60</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+      <c r="D74">
+        <v>8736</v>
+      </c>
+      <c r="E74">
+        <v>96</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>48</v>
+      </c>
+      <c r="C75">
+        <v>-12</v>
+      </c>
+      <c r="D75">
+        <v>8832</v>
+      </c>
+      <c r="E75">
+        <v>96</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>52</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76">
+        <v>8928</v>
+      </c>
+      <c r="E76">
+        <v>96</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>55</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>9024</v>
+      </c>
+      <c r="E77">
+        <v>96</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>60</v>
+      </c>
+      <c r="C78">
+        <v>5</v>
+      </c>
+      <c r="D78">
+        <v>9120</v>
+      </c>
+      <c r="E78">
+        <v>96</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>48</v>
+      </c>
+      <c r="C79">
+        <v>-12</v>
+      </c>
+      <c r="D79">
+        <v>9216</v>
+      </c>
+      <c r="E79">
+        <v>128</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>52</v>
+      </c>
+      <c r="C80">
+        <v>4</v>
+      </c>
+      <c r="D80">
+        <v>9344</v>
+      </c>
+      <c r="E80">
+        <v>128</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>55</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81">
+        <v>9472</v>
+      </c>
+      <c r="E81">
+        <v>128</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>48</v>
+      </c>
+      <c r="C82">
+        <v>-7</v>
+      </c>
+      <c r="D82">
+        <v>9600</v>
+      </c>
+      <c r="E82">
+        <v>64</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>52</v>
+      </c>
+      <c r="C83">
+        <v>4</v>
+      </c>
+      <c r="D83">
+        <v>9664</v>
+      </c>
+      <c r="E83">
+        <v>64</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>55</v>
+      </c>
+      <c r="C84">
+        <v>3</v>
+      </c>
+      <c r="D84">
+        <v>9728</v>
+      </c>
+      <c r="E84">
+        <v>64</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>48</v>
+      </c>
+      <c r="C85">
+        <v>-7</v>
+      </c>
+      <c r="D85">
+        <v>9792</v>
+      </c>
+      <c r="E85">
+        <v>32</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>52</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
+      </c>
+      <c r="D86">
+        <v>9824</v>
+      </c>
+      <c r="E86">
+        <v>32</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>55</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>9856</v>
+      </c>
+      <c r="E87">
+        <v>32</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>48</v>
+      </c>
+      <c r="C88">
+        <v>-7</v>
+      </c>
+      <c r="D88">
+        <v>9888</v>
+      </c>
+      <c r="E88">
+        <v>32</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>52</v>
+      </c>
+      <c r="C89">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <v>9920</v>
+      </c>
+      <c r="E89">
+        <v>32</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>55</v>
+      </c>
+      <c r="C90">
+        <v>3</v>
+      </c>
+      <c r="D90">
+        <v>9952</v>
+      </c>
+      <c r="E90">
+        <v>32</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>48</v>
+      </c>
+      <c r="C91">
+        <v>-7</v>
+      </c>
+      <c r="D91">
+        <v>9984</v>
+      </c>
+      <c r="E91">
+        <v>96</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="D92">
+        <v>10080</v>
+      </c>
+      <c r="E92">
+        <v>288</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>48</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>10368</v>
+      </c>
+      <c r="E93">
+        <v>48</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>52</v>
+      </c>
+      <c r="C94">
+        <v>4</v>
+      </c>
+      <c r="D94">
+        <v>10416</v>
+      </c>
+      <c r="E94">
+        <v>48</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>55</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95">
+        <v>10464</v>
+      </c>
+      <c r="E95">
+        <v>48</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>60</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
+      </c>
+      <c r="D96">
+        <v>10512</v>
+      </c>
+      <c r="E96">
+        <v>48</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>48</v>
+      </c>
+      <c r="C97">
+        <v>-12</v>
+      </c>
+      <c r="D97">
+        <v>10560</v>
+      </c>
+      <c r="E97">
+        <v>48</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>52</v>
+      </c>
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98">
+        <v>10608</v>
+      </c>
+      <c r="E98">
+        <v>48</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>59</v>
+      </c>
+      <c r="C99">
+        <v>7</v>
+      </c>
+      <c r="D99">
+        <v>10656</v>
+      </c>
+      <c r="E99">
+        <v>48</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>60</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>10704</v>
+      </c>
+      <c r="E100">
+        <v>48</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>48</v>
+      </c>
+      <c r="C101">
+        <v>-12</v>
+      </c>
+      <c r="D101">
+        <v>10752</v>
+      </c>
+      <c r="E101">
+        <v>48</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>53</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
+      </c>
+      <c r="D102">
+        <v>10800</v>
+      </c>
+      <c r="E102">
+        <v>48</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>52</v>
+      </c>
+      <c r="C103">
+        <v>-1</v>
+      </c>
+      <c r="D103">
+        <v>10848</v>
+      </c>
+      <c r="E103">
+        <v>48</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>57</v>
+      </c>
+      <c r="C104">
+        <v>5</v>
+      </c>
+      <c r="D104">
+        <v>10896</v>
+      </c>
+      <c r="E104">
+        <v>48</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>55</v>
+      </c>
+      <c r="C105">
+        <v>-2</v>
+      </c>
+      <c r="D105">
+        <v>10944</v>
+      </c>
+      <c r="E105">
+        <v>48</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>59</v>
+      </c>
+      <c r="C106">
+        <v>4</v>
+      </c>
+      <c r="D106">
+        <v>10992</v>
+      </c>
+      <c r="E106">
+        <v>48</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <v>57</v>
+      </c>
+      <c r="C107">
+        <v>-2</v>
+      </c>
+      <c r="D107">
+        <v>11040</v>
+      </c>
+      <c r="E107">
+        <v>48</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <v>60</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
+      </c>
+      <c r="D108">
+        <v>11088</v>
+      </c>
+      <c r="E108">
+        <v>48</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <v>48</v>
+      </c>
+      <c r="C109">
+        <v>-12</v>
+      </c>
+      <c r="D109">
+        <v>11136</v>
+      </c>
+      <c r="E109">
+        <v>24</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>50</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+      <c r="D110">
+        <v>11160</v>
+      </c>
+      <c r="E110">
+        <v>24</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>52</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111">
+        <v>11184</v>
+      </c>
+      <c r="E111">
+        <v>24</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <v>53</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <v>11208</v>
+      </c>
+      <c r="E112">
+        <v>24</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>55</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113">
+        <v>11232</v>
+      </c>
+      <c r="E113">
+        <v>24</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <v>57</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+      <c r="D114">
+        <v>11256</v>
+      </c>
+      <c r="E114">
+        <v>24</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115">
+        <v>59</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
+      </c>
+      <c r="D115">
+        <v>11280</v>
+      </c>
+      <c r="E115">
+        <v>24</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <v>60</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>11304</v>
+      </c>
+      <c r="E116">
+        <v>24</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <v>62</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <v>11328</v>
+      </c>
+      <c r="E117">
+        <v>24</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="G117">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <v>64</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <v>11352</v>
+      </c>
+      <c r="E118">
+        <v>24</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119">
+        <v>65</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <v>11376</v>
+      </c>
+      <c r="E119">
+        <v>24</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120">
+        <v>67</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120">
+        <v>11400</v>
+      </c>
+      <c r="E120">
+        <v>24</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121">
+        <v>69</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
+      </c>
+      <c r="D121">
+        <v>11424</v>
+      </c>
+      <c r="E121">
+        <v>24</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122">
+        <v>71</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <v>11448</v>
+      </c>
+      <c r="E122">
+        <v>24</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="G122">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <v>72</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>11472</v>
+      </c>
+      <c r="E123">
+        <v>24</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+      <c r="G123">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="D124">
+        <v>11496</v>
+      </c>
+      <c r="E124">
+        <v>24</v>
+      </c>
+      <c r="F124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125">
+        <v>48</v>
+      </c>
+      <c r="C125">
+        <v>-24</v>
+      </c>
+      <c r="D125">
+        <v>11520</v>
+      </c>
+      <c r="E125">
+        <v>24</v>
+      </c>
+      <c r="F125">
+        <v>0</v>
+      </c>
+      <c r="G125">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <v>47</v>
+      </c>
+      <c r="C126">
+        <v>-1</v>
+      </c>
+      <c r="D126">
+        <v>11544</v>
+      </c>
+      <c r="E126">
+        <v>24</v>
+      </c>
+      <c r="F126">
+        <v>0</v>
+      </c>
+      <c r="G126">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127">
+        <v>46</v>
+      </c>
+      <c r="C127">
+        <v>-1</v>
+      </c>
+      <c r="D127">
+        <v>11568</v>
+      </c>
+      <c r="E127">
+        <v>24</v>
+      </c>
+      <c r="F127">
+        <v>0</v>
+      </c>
+      <c r="G127">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128">
+        <v>45</v>
+      </c>
+      <c r="C128">
+        <v>-1</v>
+      </c>
+      <c r="D128">
+        <v>11592</v>
+      </c>
+      <c r="E128">
+        <v>24</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+      <c r="G128">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <v>44</v>
+      </c>
+      <c r="C129">
+        <v>-1</v>
+      </c>
+      <c r="D129">
+        <v>11616</v>
+      </c>
+      <c r="E129">
+        <v>24</v>
+      </c>
+      <c r="F129">
+        <v>0</v>
+      </c>
+      <c r="G129">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <v>43</v>
+      </c>
+      <c r="C130">
+        <v>-1</v>
+      </c>
+      <c r="D130">
+        <v>11640</v>
+      </c>
+      <c r="E130">
+        <v>24</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <v>42</v>
+      </c>
+      <c r="C131">
+        <v>-1</v>
+      </c>
+      <c r="D131">
+        <v>11664</v>
+      </c>
+      <c r="E131">
+        <v>24</v>
+      </c>
+      <c r="F131">
+        <v>0</v>
+      </c>
+      <c r="G131">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <v>41</v>
+      </c>
+      <c r="C132">
+        <v>-1</v>
+      </c>
+      <c r="D132">
+        <v>11688</v>
+      </c>
+      <c r="E132">
+        <v>24</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+      <c r="G132">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <v>40</v>
+      </c>
+      <c r="C133">
+        <v>-1</v>
+      </c>
+      <c r="D133">
+        <v>11712</v>
+      </c>
+      <c r="E133">
+        <v>24</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+      <c r="G133">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <v>41</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>11736</v>
+      </c>
+      <c r="E134">
+        <v>24</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+      <c r="G134">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <v>43</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <v>11760</v>
+      </c>
+      <c r="E135">
+        <v>24</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+      <c r="G135">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <v>45</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <v>11784</v>
+      </c>
+      <c r="E136">
+        <v>24</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+      <c r="G136">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>47</v>
+      </c>
+      <c r="C137">
+        <v>2</v>
+      </c>
+      <c r="D137">
+        <v>11808</v>
+      </c>
+      <c r="E137">
+        <v>24</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="G137">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <v>48</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <v>11832</v>
+      </c>
+      <c r="E138">
+        <v>24</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+      <c r="G138">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <v>50</v>
+      </c>
+      <c r="C139">
+        <v>2</v>
+      </c>
+      <c r="D139">
+        <v>11856</v>
+      </c>
+      <c r="E139">
+        <v>24</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <v>49</v>
+      </c>
+      <c r="C140">
+        <v>-1</v>
+      </c>
+      <c r="D140">
+        <v>11880</v>
+      </c>
+      <c r="E140">
+        <v>24</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <v>48</v>
+      </c>
+      <c r="C141">
+        <v>-1</v>
+      </c>
+      <c r="D141">
+        <v>11904</v>
+      </c>
+      <c r="E141">
+        <v>96</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="G141">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>52</v>
+      </c>
+      <c r="C142">
+        <v>4</v>
+      </c>
+      <c r="D142">
+        <v>12000</v>
+      </c>
+      <c r="E142">
+        <v>96</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <v>55</v>
+      </c>
+      <c r="C143">
+        <v>3</v>
+      </c>
+      <c r="D143">
+        <v>12096</v>
+      </c>
+      <c r="E143">
+        <v>96</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>60</v>
+      </c>
+      <c r="C144">
+        <v>5</v>
+      </c>
+      <c r="D144">
+        <v>12192</v>
+      </c>
+      <c r="E144">
+        <v>96</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>48</v>
+      </c>
+      <c r="C145">
+        <v>-12</v>
+      </c>
+      <c r="D145">
+        <v>12288</v>
+      </c>
+      <c r="E145">
+        <v>96</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>144</v>
+      </c>
+      <c r="B146">
+        <v>52</v>
+      </c>
+      <c r="C146">
+        <v>4</v>
+      </c>
+      <c r="D146">
+        <v>12384</v>
+      </c>
+      <c r="E146">
+        <v>96</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>145</v>
+      </c>
+      <c r="B147">
+        <v>55</v>
+      </c>
+      <c r="C147">
+        <v>3</v>
+      </c>
+      <c r="D147">
+        <v>12480</v>
+      </c>
+      <c r="E147">
+        <v>96</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+      <c r="G147">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>146</v>
+      </c>
+      <c r="B148">
+        <v>60</v>
+      </c>
+      <c r="C148">
+        <v>5</v>
+      </c>
+      <c r="D148">
+        <v>12576</v>
+      </c>
+      <c r="E148">
+        <v>96</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+      <c r="G148">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <v>48</v>
+      </c>
+      <c r="C149">
+        <v>-12</v>
+      </c>
+      <c r="D149">
+        <v>12672</v>
+      </c>
+      <c r="E149">
+        <v>96</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+      <c r="G149">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <v>52</v>
+      </c>
+      <c r="C150">
+        <v>4</v>
+      </c>
+      <c r="D150">
+        <v>12768</v>
+      </c>
+      <c r="E150">
+        <v>96</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <v>55</v>
+      </c>
+      <c r="C151">
+        <v>3</v>
+      </c>
+      <c r="D151">
+        <v>12864</v>
+      </c>
+      <c r="E151">
+        <v>96</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+      <c r="G151">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>150</v>
+      </c>
+      <c r="B152">
+        <v>60</v>
+      </c>
+      <c r="C152">
+        <v>5</v>
+      </c>
+      <c r="D152">
+        <v>12960</v>
+      </c>
+      <c r="E152">
+        <v>96</v>
+      </c>
+      <c r="F152">
+        <v>0</v>
+      </c>
+      <c r="G152">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>151</v>
+      </c>
+      <c r="B153">
+        <v>48</v>
+      </c>
+      <c r="C153">
+        <v>-12</v>
+      </c>
+      <c r="D153">
+        <v>13056</v>
+      </c>
+      <c r="E153">
+        <v>96</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>152</v>
+      </c>
+      <c r="B154">
+        <v>52</v>
+      </c>
+      <c r="C154">
+        <v>4</v>
+      </c>
+      <c r="D154">
+        <v>13152</v>
+      </c>
+      <c r="E154">
+        <v>96</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+      <c r="G154">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>153</v>
+      </c>
+      <c r="B155">
+        <v>55</v>
+      </c>
+      <c r="C155">
+        <v>3</v>
+      </c>
+      <c r="D155">
+        <v>13248</v>
+      </c>
+      <c r="E155">
+        <v>96</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="G155">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>154</v>
+      </c>
+      <c r="B156">
+        <v>60</v>
+      </c>
+      <c r="C156">
+        <v>5</v>
+      </c>
+      <c r="D156">
+        <v>13344</v>
+      </c>
+      <c r="E156">
+        <v>96</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="G156">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>155</v>
+      </c>
+      <c r="B157">
+        <v>48</v>
+      </c>
+      <c r="C157">
+        <v>-12</v>
+      </c>
+      <c r="D157">
+        <v>13440</v>
+      </c>
+      <c r="E157">
+        <v>96</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>156</v>
+      </c>
+      <c r="B158">
+        <v>52</v>
+      </c>
+      <c r="C158">
+        <v>4</v>
+      </c>
+      <c r="D158">
+        <v>13536</v>
+      </c>
+      <c r="E158">
+        <v>96</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+      <c r="G158">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>157</v>
+      </c>
+      <c r="B159">
+        <v>55</v>
+      </c>
+      <c r="C159">
+        <v>3</v>
+      </c>
+      <c r="D159">
+        <v>13632</v>
+      </c>
+      <c r="E159">
+        <v>96</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="G159">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>158</v>
+      </c>
+      <c r="B160">
+        <v>60</v>
+      </c>
+      <c r="C160">
+        <v>5</v>
+      </c>
+      <c r="D160">
+        <v>13728</v>
+      </c>
+      <c r="E160">
+        <v>96</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+      <c r="G160">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>159</v>
+      </c>
+      <c r="B161">
+        <v>48</v>
+      </c>
+      <c r="C161">
+        <v>-12</v>
+      </c>
+      <c r="D161">
+        <v>13824</v>
+      </c>
+      <c r="E161">
+        <v>96</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+      <c r="G161">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>160</v>
+      </c>
+      <c r="B162">
+        <v>52</v>
+      </c>
+      <c r="C162">
+        <v>4</v>
+      </c>
+      <c r="D162">
+        <v>13920</v>
+      </c>
+      <c r="E162">
+        <v>96</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+      <c r="G162">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>161</v>
+      </c>
+      <c r="B163">
+        <v>55</v>
+      </c>
+      <c r="C163">
+        <v>3</v>
+      </c>
+      <c r="D163">
+        <v>14016</v>
+      </c>
+      <c r="E163">
+        <v>96</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+      <c r="G163">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>162</v>
+      </c>
+      <c r="B164">
+        <v>60</v>
+      </c>
+      <c r="C164">
+        <v>5</v>
+      </c>
+      <c r="D164">
+        <v>14112</v>
+      </c>
+      <c r="E164">
+        <v>96</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+      <c r="G164">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>163</v>
+      </c>
+      <c r="B165">
+        <v>48</v>
+      </c>
+      <c r="C165">
+        <v>-12</v>
+      </c>
+      <c r="D165">
+        <v>14208</v>
+      </c>
+      <c r="E165">
+        <v>96</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="G165">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>164</v>
+      </c>
+      <c r="B166">
+        <v>52</v>
+      </c>
+      <c r="C166">
+        <v>4</v>
+      </c>
+      <c r="D166">
+        <v>14304</v>
+      </c>
+      <c r="E166">
+        <v>96</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="G166">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>165</v>
+      </c>
+      <c r="B167">
+        <v>55</v>
+      </c>
+      <c r="C167">
+        <v>3</v>
+      </c>
+      <c r="D167">
+        <v>14400</v>
+      </c>
+      <c r="E167">
+        <v>96</v>
+      </c>
+      <c r="F167">
+        <v>0</v>
+      </c>
+      <c r="G167">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>166</v>
+      </c>
+      <c r="B168">
+        <v>60</v>
+      </c>
+      <c r="C168">
+        <v>5</v>
+      </c>
+      <c r="D168">
+        <v>14496</v>
+      </c>
+      <c r="E168">
+        <v>96</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="G168">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>167</v>
+      </c>
+      <c r="B169">
+        <v>48</v>
+      </c>
+      <c r="C169">
+        <v>-12</v>
+      </c>
+      <c r="D169">
+        <v>14592</v>
+      </c>
+      <c r="E169">
+        <v>96</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+      <c r="G169">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>168</v>
+      </c>
+      <c r="B170">
+        <v>52</v>
+      </c>
+      <c r="C170">
+        <v>4</v>
+      </c>
+      <c r="D170">
+        <v>14688</v>
+      </c>
+      <c r="E170">
+        <v>96</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+      <c r="G170">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>169</v>
+      </c>
+      <c r="B171">
+        <v>55</v>
+      </c>
+      <c r="C171">
+        <v>3</v>
+      </c>
+      <c r="D171">
+        <v>14784</v>
+      </c>
+      <c r="E171">
+        <v>96</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+      <c r="G171">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>170</v>
+      </c>
+      <c r="B172">
+        <v>60</v>
+      </c>
+      <c r="C172">
+        <v>5</v>
+      </c>
+      <c r="D172">
+        <v>14880</v>
+      </c>
+      <c r="E172">
+        <v>96</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+      <c r="G172">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>171</v>
+      </c>
+      <c r="B173">
+        <v>48</v>
+      </c>
+      <c r="C173">
+        <v>-12</v>
+      </c>
+      <c r="D173">
+        <v>14976</v>
+      </c>
+      <c r="E173">
+        <v>96</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+      <c r="G173">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>172</v>
+      </c>
+      <c r="B174">
+        <v>52</v>
+      </c>
+      <c r="C174">
+        <v>4</v>
+      </c>
+      <c r="D174">
+        <v>15072</v>
+      </c>
+      <c r="E174">
+        <v>96</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+      <c r="G174">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>173</v>
+      </c>
+      <c r="B175">
+        <v>55</v>
+      </c>
+      <c r="C175">
+        <v>3</v>
+      </c>
+      <c r="D175">
+        <v>15168</v>
+      </c>
+      <c r="E175">
+        <v>96</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+      <c r="G175">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>174</v>
+      </c>
+      <c r="B176">
+        <v>60</v>
+      </c>
+      <c r="C176">
+        <v>5</v>
+      </c>
+      <c r="D176">
+        <v>15264</v>
+      </c>
+      <c r="E176">
+        <v>96</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="G176">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>175</v>
+      </c>
+      <c r="B177">
+        <v>48</v>
+      </c>
+      <c r="C177">
+        <v>-12</v>
+      </c>
+      <c r="D177">
+        <v>15360</v>
+      </c>
+      <c r="E177">
+        <v>96</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+      <c r="G177">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>176</v>
+      </c>
+      <c r="B178">
+        <v>52</v>
+      </c>
+      <c r="C178">
+        <v>4</v>
+      </c>
+      <c r="D178">
+        <v>15456</v>
+      </c>
+      <c r="E178">
+        <v>96</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="G178">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>177</v>
+      </c>
+      <c r="B179">
+        <v>55</v>
+      </c>
+      <c r="C179">
+        <v>3</v>
+      </c>
+      <c r="D179">
+        <v>15552</v>
+      </c>
+      <c r="E179">
+        <v>96</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="G179">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>178</v>
+      </c>
+      <c r="B180">
+        <v>60</v>
+      </c>
+      <c r="C180">
+        <v>5</v>
+      </c>
+      <c r="D180">
+        <v>15648</v>
+      </c>
+      <c r="E180">
+        <v>96</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="G180">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>179</v>
+      </c>
+      <c r="B181">
+        <v>48</v>
+      </c>
+      <c r="C181">
+        <v>-12</v>
+      </c>
+      <c r="D181">
+        <v>15744</v>
+      </c>
+      <c r="E181">
+        <v>96</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+      <c r="G181">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>180</v>
+      </c>
+      <c r="B182">
+        <v>52</v>
+      </c>
+      <c r="C182">
+        <v>4</v>
+      </c>
+      <c r="D182">
+        <v>15840</v>
+      </c>
+      <c r="E182">
+        <v>96</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="G182">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>181</v>
+      </c>
+      <c r="B183">
+        <v>55</v>
+      </c>
+      <c r="C183">
+        <v>3</v>
+      </c>
+      <c r="D183">
+        <v>15936</v>
+      </c>
+      <c r="E183">
+        <v>96</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>182</v>
+      </c>
+      <c r="B184">
+        <v>60</v>
+      </c>
+      <c r="C184">
+        <v>5</v>
+      </c>
+      <c r="D184">
+        <v>16032</v>
+      </c>
+      <c r="E184">
+        <v>95</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD84E5A-1FD4-43E1-98FA-38EFDF047C5B}">
   <dimension ref="A1:M184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>

</xml_diff>